<commit_message>
optimization code with lp_solve completely working. returns top N teams. fully integrated with our model output as well.
</commit_message>
<xml_diff>
--- a/RECORDS/summary.xlsx
+++ b/RECORDS/summary.xlsx
@@ -1451,7 +1451,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1506,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G9" si="0">E2-$D$2</f>
+        <f t="shared" ref="G2:G10" si="0">E2-$D$2</f>
         <v>-103</v>
       </c>
       <c r="H2">
@@ -1529,7 +1529,7 @@
         <v>880.67</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E9" si="1">D3-B3+F3+C3</f>
+        <f t="shared" ref="E3:E10" si="1">D3-B3+F3+C3</f>
         <v>843.67</v>
       </c>
       <c r="F3">
@@ -1540,7 +1540,7 @@
         <v>-140</v>
       </c>
       <c r="H3" s="7">
-        <f t="shared" ref="H3:H9" si="2">E3/$D$2</f>
+        <f t="shared" ref="H3:H10" si="2">E3/$D$2</f>
         <v>0.85767584657456264</v>
       </c>
     </row>
@@ -1555,7 +1555,7 @@
         <v>235.8</v>
       </c>
       <c r="D4" s="7">
-        <f t="shared" ref="D4:D9" si="3">E3</f>
+        <f t="shared" ref="D4:D10" si="3">E3</f>
         <v>843.67</v>
       </c>
       <c r="E4" s="7">
@@ -1725,8 +1725,26 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="1">
+        <v>41971</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="3"/>
+        <v>845.57</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>845.57</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>-138.09999999999991</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="2"/>
+        <v>0.859607388656765</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added aliasing so people can have multiple names ie kj mcdaniels; added minutes lever into possessions model
</commit_message>
<xml_diff>
--- a/RECORDS/summary.xlsx
+++ b/RECORDS/summary.xlsx
@@ -505,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -560,22 +560,22 @@
         <v>983.67</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E14" si="0">D2-B2+F2+C2</f>
+        <f t="shared" ref="E2:E20" si="0">D2-B2+F2+C2</f>
         <v>880.67</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
       <c r="G2" s="7">
-        <f t="shared" ref="G2:G14" si="1">E2-D2</f>
+        <f t="shared" ref="G2:G20" si="1">E2-D2</f>
         <v>-103</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H14" si="2">E2-$D$2</f>
+        <f t="shared" ref="H2:H20" si="2">E2-$D$2</f>
         <v>-103</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I14" si="3">E2/$D$2</f>
+        <f t="shared" ref="I2:I20" si="3">E2/$D$2</f>
         <v>0.89529008712271396</v>
       </c>
     </row>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D14" si="4">E2</f>
+        <f t="shared" ref="D3:D20" si="4">E2</f>
         <v>880.67</v>
       </c>
       <c r="E3" s="7">
@@ -985,6 +985,165 @@
       <c r="I14" s="7">
         <f t="shared" si="3"/>
         <v>0.74310490306708554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>41976</v>
+      </c>
+      <c r="B15">
+        <v>122</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="4"/>
+        <v>730.97</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>613.97</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="1"/>
+        <v>-117</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="2"/>
+        <v>-369.69999999999993</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="3"/>
+        <v>0.62416257484725579</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>41977</v>
+      </c>
+      <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16">
+        <v>5.4</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="4"/>
+        <v>613.97</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>558.37</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="1"/>
+        <v>-55.600000000000023</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="2"/>
+        <v>-425.29999999999995</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="3"/>
+        <v>0.56763955391543919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>41978</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="4"/>
+        <v>558.37</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>558.37</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="2"/>
+        <v>-425.29999999999995</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="3"/>
+        <v>0.56763955391543919</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D18" s="7">
+        <f t="shared" si="4"/>
+        <v>558.37</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>558.37</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="2"/>
+        <v>-425.29999999999995</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="3"/>
+        <v>0.56763955391543919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D19" s="7">
+        <f t="shared" si="4"/>
+        <v>558.37</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>558.37</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="7">
+        <f t="shared" si="2"/>
+        <v>-425.29999999999995</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="3"/>
+        <v>0.56763955391543919</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D20" s="7">
+        <f t="shared" si="4"/>
+        <v>558.37</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>558.37</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="2"/>
+        <v>-425.29999999999995</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="3"/>
+        <v>0.56763955391543919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code to see how often a player is recommended
</commit_message>
<xml_diff>
--- a/RECORDS/summary.xlsx
+++ b/RECORDS/summary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -131,24 +131,6 @@
   </si>
   <si>
     <t>Daily Total</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Refund for Cancelled Contest</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Entry Fee</t>
-  </si>
-  <si>
-    <t>Contest Entry Fee</t>
   </si>
   <si>
     <t>Daily PnL</t>
@@ -505,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -540,10 +522,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
@@ -560,22 +542,22 @@
         <v>983.67</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E20" si="0">D2-B2+F2+C2</f>
+        <f t="shared" ref="E2:E23" si="0">D2-B2+F2+C2</f>
         <v>880.67</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
       <c r="G2" s="7">
-        <f t="shared" ref="G2:G20" si="1">E2-D2</f>
+        <f t="shared" ref="G2:G23" si="1">E2-D2</f>
         <v>-103</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H20" si="2">E2-$D$2</f>
+        <f t="shared" ref="H2:H23" si="2">E2-$D$2</f>
         <v>-103</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I20" si="3">E2/$D$2</f>
+        <f t="shared" ref="I2:I23" si="3">E2/$D$2</f>
         <v>0.89529008712271396</v>
       </c>
     </row>
@@ -590,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D20" si="4">E2</f>
+        <f t="shared" ref="D3:D23" si="4">E2</f>
         <v>880.67</v>
       </c>
       <c r="E3" s="7">
@@ -877,7 +859,7 @@
         <v>83.199999999999932</v>
       </c>
       <c r="H11" s="7">
-        <f>E11-$D$2</f>
+        <f t="shared" si="2"/>
         <v>-137.89999999999998</v>
       </c>
       <c r="I11" s="7">
@@ -1059,91 +1041,218 @@
       <c r="A17" s="1">
         <v>41978</v>
       </c>
+      <c r="B17">
+        <v>163</v>
+      </c>
+      <c r="C17">
+        <v>2.7</v>
+      </c>
       <c r="D17" s="7">
         <f t="shared" si="4"/>
         <v>558.37</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>558.37</v>
+        <v>404.07</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-154.30000000000001</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" si="2"/>
-        <v>-425.29999999999995</v>
+        <v>-579.59999999999991</v>
       </c>
       <c r="I17" s="7">
         <f t="shared" si="3"/>
-        <v>0.56763955391543919</v>
+        <v>0.4107780048186892</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>41979</v>
+      </c>
+      <c r="B18">
+        <f>89+14*3+9*5</f>
+        <v>176</v>
+      </c>
+      <c r="C18">
+        <v>291.60000000000002</v>
+      </c>
       <c r="D18" s="7">
         <f t="shared" si="4"/>
-        <v>558.37</v>
+        <v>404.07</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>558.37</v>
+        <v>526.67000000000007</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>122.60000000000008</v>
       </c>
       <c r="H18" s="7">
         <f t="shared" si="2"/>
-        <v>-425.29999999999995</v>
+        <v>-456.99999999999989</v>
       </c>
       <c r="I18" s="7">
         <f t="shared" si="3"/>
-        <v>0.56763955391543919</v>
+        <v>0.53541329917553659</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>41980</v>
+      </c>
+      <c r="B19">
+        <v>110</v>
+      </c>
+      <c r="C19">
+        <v>0.9</v>
+      </c>
       <c r="D19" s="7">
         <f t="shared" si="4"/>
-        <v>558.37</v>
+        <v>526.67000000000007</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
-        <v>558.37</v>
+        <v>421.57000000000005</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-105.10000000000002</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" si="2"/>
-        <v>-425.29999999999995</v>
+        <v>-562.09999999999991</v>
       </c>
       <c r="I19" s="7">
         <f t="shared" si="3"/>
-        <v>0.56763955391543919</v>
+        <v>0.42856852399686896</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>41981</v>
+      </c>
+      <c r="B20">
+        <v>104</v>
+      </c>
+      <c r="C20">
+        <v>153.9</v>
+      </c>
       <c r="D20" s="7">
         <f t="shared" si="4"/>
-        <v>558.37</v>
+        <v>421.57000000000005</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>558.37</v>
+        <v>475.47</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>53.899999999999977</v>
       </c>
       <c r="H20" s="7">
         <f t="shared" si="2"/>
-        <v>-425.29999999999995</v>
+        <v>-508.19999999999993</v>
       </c>
       <c r="I20" s="7">
         <f t="shared" si="3"/>
-        <v>0.56763955391543919</v>
+        <v>0.48336332306566232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>41982</v>
+      </c>
+      <c r="B21">
+        <v>113</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="4"/>
+        <v>475.47</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>366.47</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="1"/>
+        <v>-109</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="2"/>
+        <v>-617.19999999999993</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="3"/>
+        <v>0.37255380361300033</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>41983</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="4"/>
+        <v>366.47</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="0"/>
+        <v>366.47</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="2"/>
+        <v>-617.19999999999993</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="3"/>
+        <v>0.37255380361300033</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>41984</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="4"/>
+        <v>366.47</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>366.47</v>
+      </c>
+      <c r="G23" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="2"/>
+        <v>-617.19999999999993</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="3"/>
+        <v>0.37255380361300033</v>
       </c>
     </row>
   </sheetData>
@@ -1156,2104 +1265,847 @@
   <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G4" sqref="A1:G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="8">
-        <v>41975.796180555553</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="10">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="4">
-        <f>SUM(C1:C28)</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="8">
-        <v>41975.796180555553</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="4">
-        <f>SUM(C29:C104)</f>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="8">
-        <v>41975.796180555553</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="4">
-        <f>G2-G1</f>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="8">
-        <v>41975.796168981484</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="8">
-        <v>41975.796168981484</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="10">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="8">
-        <v>41975.794259259259</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="8">
-        <v>41975.794259259259</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="10">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="8">
-        <v>41975.794247685182</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="8">
-        <v>41975.794247685182</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="8">
-        <v>41975.794247685182</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A11" s="8">
-        <v>41975.794236111113</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="8">
-        <v>41975.794236111113</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="8">
-        <v>41975.794224537036</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="10">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="8">
-        <v>41975.794224537036</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A15" s="8">
-        <v>41975.794212962966</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A16" s="8">
-        <v>41975.794212962966</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="8">
-        <v>41975.79420138889</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="10">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A18" s="8">
-        <v>41975.794189814813</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="10">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A19" s="8">
-        <v>41975.70989583333</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="10">
-        <v>10</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="8">
-        <v>41975.709675925929</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="10">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A21" s="8">
-        <v>41975.709537037037</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="10">
-        <v>5</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="8">
-        <v>41975.709421296298</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="10">
-        <v>5</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A23" s="8">
-        <v>41975.70921296296</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="10">
-        <v>5</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="8">
-        <v>41975.709074074075</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="10">
-        <v>3</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="8">
-        <v>41975.70894675926</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="10">
-        <v>5</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A26" s="8">
-        <v>41975.708807870367</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="10">
-        <v>5</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A27" s="8">
-        <v>41975.70857638889</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="10">
-        <v>10</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A28" s="8">
-        <v>41975.708356481482</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="10">
-        <v>10</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="8">
-        <v>41975.707766203705</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="10">
-        <v>10</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="8">
-        <v>41975.707766203705</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="10">
-        <v>5</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>38</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="8">
-        <v>41975.707766203705</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="10">
-        <v>5</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>38</v>
-      </c>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="8">
-        <v>41975.707766203705</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="10">
-        <v>5</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="8">
-        <v>41975.707766203705</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="10">
-        <v>5</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="10">
-        <v>10</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="10">
-        <v>10</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="10">
-        <v>10</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="10">
-        <v>5</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="10">
-        <v>5</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="10">
-        <v>5</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="10">
-        <v>5</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="10">
-        <v>5</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="10">
-        <v>5</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="10">
-        <v>5</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A44" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="10">
-        <v>5</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="10">
-        <v>5</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A46" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="10">
-        <v>3</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="10">
-        <v>3</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A48" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="10">
-        <v>3</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" s="10">
-        <v>3</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="10">
-        <v>3</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="10">
-        <v>3</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A52" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C52" s="10">
-        <v>3</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A53" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" s="10">
-        <v>3</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="10">
-        <v>3</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A55" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C55" s="10">
-        <v>3</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A56" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="10">
-        <v>3</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A57" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="10">
-        <v>3</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A58" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="10">
-        <v>3</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A59" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="10">
-        <v>3</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A60" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" s="10">
-        <v>1</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A61" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="10">
-        <v>1</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A62" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" s="10">
-        <v>1</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A63" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C63" s="10">
-        <v>1</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A64" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C64" s="10">
-        <v>1</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A65" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65" s="10">
-        <v>1</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A66" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C66" s="10">
-        <v>1</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A67" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" s="10">
-        <v>1</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A68" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C68" s="10">
-        <v>1</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A69" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C69" s="10">
-        <v>1</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A70" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C70" s="10">
-        <v>1</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A71" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C71" s="10">
-        <v>1</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A72" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C72" s="10">
-        <v>1</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A73" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C73" s="10">
-        <v>1</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A74" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C74" s="10">
-        <v>1</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A75" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C75" s="10">
-        <v>1</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A76" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="10">
-        <v>1</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A77" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C77" s="10">
-        <v>1</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A78" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C78" s="10">
-        <v>1</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A79" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C79" s="10">
-        <v>1</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A80" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C80" s="10">
-        <v>1</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A81" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C81" s="10">
-        <v>1</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A82" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C82" s="10">
-        <v>1</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A83" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C83" s="10">
-        <v>1</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A84" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C84" s="10">
-        <v>1</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A85" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C85" s="10">
-        <v>1</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A86" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C86" s="10">
-        <v>1</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A87" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C87" s="10">
-        <v>1</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A88" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C88" s="10">
-        <v>1</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A89" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C89" s="10">
-        <v>1</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A90" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C90" s="10">
-        <v>1</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A91" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C91" s="10">
-        <v>1</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A92" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C92" s="10">
-        <v>1</v>
-      </c>
-      <c r="D92" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A93" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C93" s="10">
-        <v>1</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A94" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C94" s="10">
-        <v>1</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A95" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C95" s="10">
-        <v>1</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A96" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C96" s="10">
-        <v>1</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A97" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C97" s="10">
-        <v>1</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A98" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C98" s="10">
-        <v>1</v>
-      </c>
-      <c r="D98" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A99" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C99" s="10">
-        <v>1</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A100" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C100" s="10">
-        <v>1</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A101" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C101" s="10">
-        <v>1</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A102" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C102" s="10">
-        <v>1</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A103" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C103" s="10">
-        <v>1</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A104" s="8">
-        <v>41975.707268518519</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C104" s="10">
-        <v>1</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>38</v>
-      </c>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="8"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="8"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="8"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="8"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="8"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="8"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="8"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="8"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="8"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="8"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="8"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="8"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="8"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="8"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="8"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" s="8"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" s="8"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A87" s="8"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A89" s="8"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A91" s="8"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A93" s="8"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A95" s="8"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A97" s="8"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" s="8"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" s="8"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" s="8"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A102" s="8"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A103" s="8"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" s="8"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixes to fppp average, minutes ewma
</commit_message>
<xml_diff>
--- a/RECORDS/summary.xlsx
+++ b/RECORDS/summary.xlsx
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1181,6 +1181,9 @@
       <c r="B21">
         <v>113</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
       <c r="D21" s="7">
         <f t="shared" si="4"/>
         <v>475.47</v>
@@ -1209,38 +1212,48 @@
       <c r="A22" s="1">
         <v>41983</v>
       </c>
+      <c r="B22">
+        <v>139</v>
+      </c>
+      <c r="C22">
+        <f>91.8</f>
+        <v>91.8</v>
+      </c>
       <c r="D22" s="7">
         <f t="shared" si="4"/>
         <v>366.47</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>366.47</v>
+        <v>325.27000000000004</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-41.199999999999989</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="2"/>
-        <v>-617.19999999999993</v>
+        <v>-658.39999999999986</v>
       </c>
       <c r="I22" s="7">
         <f t="shared" si="3"/>
-        <v>0.37255380361300033</v>
+        <v>0.33066983846208592</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
-        <v>41984</v>
+        <v>41985</v>
       </c>
       <c r="D23" s="7">
         <f t="shared" si="4"/>
-        <v>366.47</v>
+        <v>325.27000000000004</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>366.47</v>
+        <v>325.27000000000004</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="1"/>
@@ -1248,11 +1261,11 @@
       </c>
       <c r="H23" s="7">
         <f t="shared" si="2"/>
-        <v>-617.19999999999993</v>
+        <v>-658.39999999999986</v>
       </c>
       <c r="I23" s="7">
         <f t="shared" si="3"/>
-        <v>0.37255380361300033</v>
+        <v>0.33066983846208592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>